<commit_message>
adding in monthly predictors for mascot glm
</commit_message>
<xml_diff>
--- a/data/mpox_geocoding.xlsx
+++ b/data/mpox_geocoding.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mparedes/Desktop/gitrepos/monkeypox-dynamics-mp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D28EA47-DB82-A241-87AF-84E7234352FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7E9510-F9EE-6B4E-B3ED-649F224B9CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{64B635B0-B386-4844-897A-1BA296BF99A9}"/>
   </bookViews>
@@ -169,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -312,11 +312,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -379,6 +444,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C1457E-31BD-8B45-B217-AB90017E6D67}">
-  <dimension ref="C1:F16"/>
+  <dimension ref="F1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F16"/>
+      <selection activeCell="F1" sqref="F1:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,213 +822,214 @@
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="8" t="s">
+    </row>
+    <row r="2" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F3" s="24"/>
+      <c r="G3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="10">
+        <v>533</v>
+      </c>
+      <c r="I3" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="12">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F5" s="26"/>
+      <c r="G5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>116</v>
+      </c>
+      <c r="I5" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F6" s="26"/>
+      <c r="G6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="12">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F7" s="26"/>
+      <c r="G7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="12">
+        <v>94</v>
+      </c>
+      <c r="I7" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F8" s="26"/>
+      <c r="G8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="12">
+        <v>25</v>
+      </c>
+      <c r="I8" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F9" s="27"/>
+      <c r="G9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="12">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F10" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="14">
         <v>0</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="10">
-        <v>27</v>
-      </c>
-      <c r="D2" s="11">
-        <v>45</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C3" s="10">
-        <v>533</v>
-      </c>
-      <c r="D3" s="11">
-        <v>120</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="I10" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F11" s="29"/>
+      <c r="G11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F12" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="16">
+        <v>6</v>
+      </c>
+      <c r="I12" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F13" s="31"/>
+      <c r="G13" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="16">
+        <v>88</v>
+      </c>
+      <c r="I13" s="4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F14" s="32"/>
+      <c r="G14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="16">
+        <v>9</v>
+      </c>
+      <c r="I14" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F15" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="18">
+        <v>77</v>
+      </c>
+      <c r="I15" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="6:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="34"/>
+      <c r="G16" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="20">
         <v>3</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="12">
-        <v>3</v>
-      </c>
-      <c r="D4" s="13">
-        <v>11</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="12">
-        <v>116</v>
-      </c>
-      <c r="D5" s="13">
-        <v>84</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="12">
-        <v>7</v>
-      </c>
-      <c r="D6" s="13">
-        <v>7</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="12">
-        <v>94</v>
-      </c>
-      <c r="D7" s="13">
-        <v>78</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C8" s="12">
-        <v>25</v>
-      </c>
-      <c r="D8" s="13">
-        <v>23</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="12">
-        <v>15</v>
-      </c>
-      <c r="D9" s="13">
-        <v>18</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="14">
-        <v>0</v>
-      </c>
-      <c r="D10" s="15">
-        <v>11</v>
-      </c>
-      <c r="E10" s="15" t="s">
+      <c r="I16" s="6">
         <v>10</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="14">
-        <v>0</v>
-      </c>
-      <c r="D11" s="15">
-        <v>31</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="16">
-        <v>6</v>
-      </c>
-      <c r="D12" s="17">
-        <v>7</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="16">
-        <v>88</v>
-      </c>
-      <c r="D13" s="17">
-        <v>75</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="16">
-        <v>9</v>
-      </c>
-      <c r="D14" s="17">
-        <v>11</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C15" s="18">
-        <v>77</v>
-      </c>
-      <c r="D15" s="19">
-        <v>57</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="20">
-        <v>3</v>
-      </c>
-      <c r="D16" s="21">
-        <v>10</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>